<commit_message>
Fixed bug in application files
Fixed bug preventing commas from working in function descriptions.  Added quit and reset buttons
</commit_message>
<xml_diff>
--- a/spreadsheet_files/Muscle_action_answer_calculator.xlsx
+++ b/spreadsheet_files/Muscle_action_answer_calculator.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pattillo/Documents/GitHub/smart-skeleton/spreadsheet_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8C058C-653F-0A47-8A22-78D890204257}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAD43014-E070-054D-B321-4F9E21B94D4B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1680" windowWidth="25600" windowHeight="13340" activeTab="2" xr2:uid="{4AB589AF-D212-FE40-8E11-EEE1EB78BB5E}"/>
+    <workbookView xWindow="0" yWindow="1700" windowWidth="25600" windowHeight="13340" activeTab="1" xr2:uid="{4AB589AF-D212-FE40-8E11-EEE1EB78BB5E}"/>
   </bookViews>
   <sheets>
     <sheet name="answer code calculator" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="150">
   <si>
     <t>Wrist abducted</t>
   </si>
@@ -491,6 +491,12 @@
   </si>
   <si>
     <t>rotation of the knee is not currently detected. Only actions on the hip should be used.</t>
+  </si>
+  <si>
+    <t>Warning!  Do not use commas in the text fields of questions.csv.  Substitute a "|" for a comma, and the application will render a comma.</t>
+  </si>
+  <si>
+    <t>For example if you want a field to say "No, please try again." then enter "No| please try again".  The text will appear with a comma on screen.</t>
   </si>
 </sst>
 </file>
@@ -877,8 +883,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3A80A61C-C86A-CA41-97C5-C95EF91DE2F5}">
   <dimension ref="A1:AN34"/>
   <sheetViews>
-    <sheetView topLeftCell="B2" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="AN7" sqref="AN7"/>
+    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="AN5" sqref="AN5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1623,10 +1629,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D745D06A-7587-3048-B8DA-EF8263E0CA9C}">
-  <dimension ref="A1:B16"/>
+  <dimension ref="A1:B20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1740,6 +1746,16 @@
         <v>137</v>
       </c>
     </row>
+    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A19" s="7" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A20" s="7" t="s">
+        <v>149</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1749,8 +1765,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3D1884C-B231-9148-BE01-A45E67A1E81D}">
   <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E75" sqref="E75"/>
+    <sheetView topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="C46" sqref="C46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2176,7 +2192,7 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
-        <v>109</v>
+        <v>61</v>
       </c>
       <c r="B45">
         <v>44</v>
@@ -2184,7 +2200,7 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>61</v>
+        <v>109</v>
       </c>
       <c r="B46">
         <v>45</v>

</xml_diff>